<commit_message>
Final preparations for defense
</commit_message>
<xml_diff>
--- a/Dissertation Backup/Interaction Figures.xlsx
+++ b/Dissertation Backup/Interaction Figures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teres\Documents\GitHub\MenidiaOA\Dissertation Backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A847AEE0-3F2B-4864-B231-4DCF359C06B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D93A11-1EB9-4F54-ACB1-A7E570443D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{591B7BEE-5214-4F17-9185-55FF80664E5C}"/>
   </bookViews>
@@ -373,6 +373,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="4.7393364928909949E-2"/>
+              <c:y val="0.40259660250801982"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4158,8 +4166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA417443-2C13-454F-8BF4-1B5723F9389D}">
   <dimension ref="A4:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>